<commit_message>
updated checkbox method for week 3 data-driven testing
</commit_message>
<xml_diff>
--- a/Week3-Data-Driven-Testing/Week3-DataDriven.xlsx
+++ b/Week3-Data-Driven-Testing/Week3-DataDriven.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>-6</t>
+  </si>
+  <si>
+    <t>SourceCodeManagement</t>
+  </si>
+  <si>
+    <t>CVS</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -446,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -457,10 +466,10 @@
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -476,8 +485,11 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -489,8 +501,11 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -506,8 +521,11 @@
       <c r="E3" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -522,7 +540,7 @@
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -537,7 +555,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>9</v>
@@ -550,7 +568,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>12</v>

</xml_diff>